<commit_message>
Update IESO report from GitHub Actions
</commit_message>
<xml_diff>
--- a/output/latest.xlsx
+++ b/output/latest.xlsx
@@ -498,7 +498,7 @@
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>CreatedAt: 2025-05-03T23:10:24</t>
+          <t>CreatedAt: 2025-05-04T00:10:44</t>
         </is>
       </c>
       <c r="B1" s="3" t="n"/>
@@ -658,13 +658,13 @@
         <v>15.1</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>99</v>
+        <v>7.04</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>155</v>
+        <v>105.2</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>155</v>
+        <v>75</v>
       </c>
       <c r="G4" s="3" t="n">
         <v>155</v>
@@ -703,19 +703,19 @@
         <v>0</v>
       </c>
       <c r="S4" s="3" t="n">
-        <v>6.04</v>
+        <v>6.17</v>
       </c>
       <c r="T4" s="3" t="n">
-        <v>6.46</v>
+        <v>6.22</v>
       </c>
       <c r="U4" s="3" t="n">
-        <v>6.29</v>
+        <v>6.18</v>
       </c>
       <c r="V4" s="3" t="n">
-        <v>6.5</v>
+        <v>6.41</v>
       </c>
       <c r="W4" s="3" t="n">
-        <v>6.19</v>
+        <v>6.21</v>
       </c>
       <c r="X4" s="3" t="n">
         <v>0</v>
@@ -826,10 +826,10 @@
         <v>0.4</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>0.11</v>
+        <v>0.23</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>0</v>
@@ -880,10 +880,10 @@
         <v>0.16</v>
       </c>
       <c r="V6" s="3" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="W6" s="3" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="X6" s="3" t="n">
         <v>0</v>
@@ -910,13 +910,13 @@
         <v>0</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>92.31999999999999</v>
+        <v>0</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>148.8</v>
+        <v>98.7</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>155</v>
+        <v>75</v>
       </c>
       <c r="G7" s="3" t="n">
         <v>155</v>
@@ -1081,7 +1081,7 @@
         <v>22.6</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>6.45</v>
+        <v>22.59</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>0</v>
@@ -1123,19 +1123,19 @@
         <v>0</v>
       </c>
       <c r="S9" s="3" t="n">
-        <v>6.19</v>
+        <v>6.33</v>
       </c>
       <c r="T9" s="3" t="n">
-        <v>6.6</v>
+        <v>6.37</v>
       </c>
       <c r="U9" s="3" t="n">
-        <v>6.44</v>
+        <v>6.34</v>
       </c>
       <c r="V9" s="3" t="n">
-        <v>6.73</v>
+        <v>6.55</v>
       </c>
       <c r="W9" s="3" t="n">
-        <v>6.35</v>
+        <v>6.38</v>
       </c>
       <c r="X9" s="3" t="n">
         <v>0</v>
@@ -1246,10 +1246,10 @@
         <v>0.77</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>0.46</v>
+        <v>0.44</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="F11" s="3" t="n">
         <v>0</v>
@@ -1291,19 +1291,19 @@
         <v>0</v>
       </c>
       <c r="S11" s="3" t="n">
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
       <c r="T11" s="3" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="U11" s="3" t="n">
         <v>0.32</v>
       </c>
-      <c r="U11" s="3" t="n">
+      <c r="V11" s="3" t="n">
         <v>0.31</v>
       </c>
-      <c r="V11" s="3" t="n">
-        <v>0.4</v>
-      </c>
       <c r="W11" s="3" t="n">
-        <v>0.32</v>
+        <v>0.33</v>
       </c>
       <c r="X11" s="3" t="n">
         <v>0</v>
@@ -1330,10 +1330,10 @@
         <v>7.14</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>15.57</v>
+        <v>15.34</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>0</v>
+        <v>15.89</v>
       </c>
       <c r="F12" s="3" t="n">
         <v>0</v>
@@ -1501,7 +1501,7 @@
         <v>22.6</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>6.45</v>
+        <v>22.6</v>
       </c>
       <c r="F14" s="3" t="n">
         <v>5.86</v>
@@ -1543,19 +1543,19 @@
         <v>5.31</v>
       </c>
       <c r="S14" s="3" t="n">
-        <v>6.19</v>
+        <v>6.33</v>
       </c>
       <c r="T14" s="3" t="n">
-        <v>6.61</v>
+        <v>6.37</v>
       </c>
       <c r="U14" s="3" t="n">
-        <v>6.44</v>
+        <v>6.34</v>
       </c>
       <c r="V14" s="3" t="n">
-        <v>6.73</v>
+        <v>6.55</v>
       </c>
       <c r="W14" s="3" t="n">
-        <v>6.35</v>
+        <v>6.39</v>
       </c>
       <c r="X14" s="3" t="n">
         <v>5.86</v>
@@ -1666,10 +1666,10 @@
         <v>0.77</v>
       </c>
       <c r="D16" s="3" t="n">
-        <v>0.46</v>
+        <v>0.44</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="F16" s="3" t="n">
         <v>0</v>
@@ -1711,19 +1711,19 @@
         <v>0</v>
       </c>
       <c r="S16" s="3" t="n">
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
       <c r="T16" s="3" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="U16" s="3" t="n">
         <v>0.32</v>
       </c>
-      <c r="U16" s="3" t="n">
+      <c r="V16" s="3" t="n">
         <v>0.31</v>
       </c>
-      <c r="V16" s="3" t="n">
-        <v>0.41</v>
-      </c>
       <c r="W16" s="3" t="n">
-        <v>0.32</v>
+        <v>0.33</v>
       </c>
       <c r="X16" s="3" t="n">
         <v>0</v>
@@ -1750,10 +1750,10 @@
         <v>7.14</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>15.57</v>
+        <v>15.34</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>0</v>
+        <v>15.89</v>
       </c>
       <c r="F17" s="3" t="n">
         <v>0</v>
@@ -1921,10 +1921,10 @@
         <v>53</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>33.94</v>
+        <v>74.95</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="G19" s="3" t="n">
         <v>32</v>
@@ -1963,13 +1963,13 @@
         <v>0</v>
       </c>
       <c r="S19" s="3" t="n">
-        <v>6.09</v>
+        <v>6.22</v>
       </c>
       <c r="T19" s="3" t="n">
-        <v>6.5</v>
+        <v>6.27</v>
       </c>
       <c r="U19" s="3" t="n">
-        <v>114.96</v>
+        <v>114.97</v>
       </c>
       <c r="V19" s="3" t="n">
         <v>114.96</v>
@@ -2086,10 +2086,10 @@
         <v>0.54</v>
       </c>
       <c r="D21" s="3" t="n">
-        <v>0.17</v>
+        <v>0.28</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="F21" s="3" t="n">
         <v>0</v>
@@ -2131,16 +2131,16 @@
         <v>0</v>
       </c>
       <c r="S21" s="3" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="T21" s="3" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="U21" s="3" t="n">
         <v>0.21</v>
       </c>
       <c r="V21" s="3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="W21" s="3" t="n">
         <v>0.21</v>
@@ -2170,13 +2170,13 @@
         <v>0</v>
       </c>
       <c r="D22" s="3" t="n">
-        <v>46.26</v>
+        <v>45.9</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>27.68</v>
+        <v>68.39</v>
       </c>
       <c r="F22" s="3" t="n">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="G22" s="3" t="n">
         <v>32</v>
@@ -2221,13 +2221,13 @@
         <v>0</v>
       </c>
       <c r="U22" s="3" t="n">
-        <v>108.62</v>
+        <v>108.73</v>
       </c>
       <c r="V22" s="3" t="n">
-        <v>108.41</v>
+        <v>108.51</v>
       </c>
       <c r="W22" s="3" t="n">
-        <v>36.72</v>
+        <v>36.7</v>
       </c>
       <c r="X22" s="3" t="n">
         <v>0</v>
@@ -2338,13 +2338,13 @@
         <v>15.23</v>
       </c>
       <c r="D24" s="3" t="n">
-        <v>99.06</v>
+        <v>7.1</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>155.06</v>
+        <v>105.26</v>
       </c>
       <c r="F24" s="3" t="n">
-        <v>155</v>
+        <v>75</v>
       </c>
       <c r="G24" s="3" t="n">
         <v>155</v>
@@ -2383,19 +2383,19 @@
         <v>0</v>
       </c>
       <c r="S24" s="3" t="n">
-        <v>6.09</v>
+        <v>6.22</v>
       </c>
       <c r="T24" s="3" t="n">
-        <v>6.5</v>
+        <v>6.27</v>
       </c>
       <c r="U24" s="3" t="n">
-        <v>6.34</v>
+        <v>6.23</v>
       </c>
       <c r="V24" s="3" t="n">
-        <v>6.55</v>
+        <v>6.45</v>
       </c>
       <c r="W24" s="3" t="n">
-        <v>6.24</v>
+        <v>6.26</v>
       </c>
       <c r="X24" s="3" t="n">
         <v>0</v>
@@ -2506,10 +2506,10 @@
         <v>0.54</v>
       </c>
       <c r="D26" s="3" t="n">
-        <v>0.17</v>
+        <v>0.28</v>
       </c>
       <c r="E26" s="3" t="n">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="F26" s="3" t="n">
         <v>0</v>
@@ -2551,16 +2551,16 @@
         <v>0</v>
       </c>
       <c r="S26" s="3" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="T26" s="3" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="U26" s="3" t="n">
         <v>0.21</v>
       </c>
       <c r="V26" s="3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="W26" s="3" t="n">
         <v>0.21</v>
@@ -2590,13 +2590,13 @@
         <v>0</v>
       </c>
       <c r="D27" s="3" t="n">
-        <v>92.31999999999999</v>
+        <v>0</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>148.8</v>
+        <v>98.7</v>
       </c>
       <c r="F27" s="3" t="n">
-        <v>155</v>
+        <v>75</v>
       </c>
       <c r="G27" s="3" t="n">
         <v>155</v>
@@ -2758,13 +2758,13 @@
         <v>15.37</v>
       </c>
       <c r="D29" s="3" t="n">
-        <v>53.05</v>
+        <v>53.06</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="F29" s="3" t="n">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="G29" s="3" t="n">
         <v>32</v>
@@ -2803,10 +2803,10 @@
         <v>0</v>
       </c>
       <c r="S29" s="3" t="n">
-        <v>6.13</v>
+        <v>6.26</v>
       </c>
       <c r="T29" s="3" t="n">
-        <v>6.54</v>
+        <v>6.31</v>
       </c>
       <c r="U29" s="3" t="n">
         <v>115</v>
@@ -2926,10 +2926,10 @@
         <v>0.67</v>
       </c>
       <c r="D31" s="3" t="n">
-        <v>0.22</v>
+        <v>0.34</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>0.31</v>
+        <v>0.32</v>
       </c>
       <c r="F31" s="3" t="n">
         <v>0</v>
@@ -2971,19 +2971,19 @@
         <v>0</v>
       </c>
       <c r="S31" s="3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="T31" s="3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="U31" s="3" t="n">
         <v>0.24</v>
       </c>
-      <c r="T31" s="3" t="n">
-        <v>0.26</v>
-      </c>
-      <c r="U31" s="3" t="n">
+      <c r="V31" s="3" t="n">
         <v>0.25</v>
       </c>
-      <c r="V31" s="3" t="n">
-        <v>0.27</v>
-      </c>
       <c r="W31" s="3" t="n">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="X31" s="3" t="n">
         <v>0</v>
@@ -3010,13 +3010,13 @@
         <v>0</v>
       </c>
       <c r="D32" s="3" t="n">
-        <v>46.26</v>
+        <v>45.9</v>
       </c>
       <c r="E32" s="3" t="n">
-        <v>27.68</v>
+        <v>68.39</v>
       </c>
       <c r="F32" s="3" t="n">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="G32" s="3" t="n">
         <v>32</v>
@@ -3061,13 +3061,13 @@
         <v>0</v>
       </c>
       <c r="U32" s="3" t="n">
-        <v>108.62</v>
+        <v>108.73</v>
       </c>
       <c r="V32" s="3" t="n">
-        <v>108.41</v>
+        <v>108.51</v>
       </c>
       <c r="W32" s="3" t="n">
-        <v>36.72</v>
+        <v>36.7</v>
       </c>
       <c r="X32" s="3" t="n">
         <v>0</v>
@@ -3181,7 +3181,7 @@
         <v>25.37</v>
       </c>
       <c r="E34" s="3" t="n">
-        <v>6.53</v>
+        <v>27</v>
       </c>
       <c r="F34" s="3" t="n">
         <v>5.86</v>
@@ -3205,10 +3205,10 @@
         <v>5.46</v>
       </c>
       <c r="M34" s="3" t="n">
-        <v>5.84</v>
+        <v>5.85</v>
       </c>
       <c r="N34" s="3" t="n">
-        <v>5.55</v>
+        <v>5.5</v>
       </c>
       <c r="O34" s="3" t="n">
         <v>25</v>
@@ -3223,19 +3223,19 @@
         <v>5.31</v>
       </c>
       <c r="S34" s="3" t="n">
-        <v>6.24</v>
+        <v>6.38</v>
       </c>
       <c r="T34" s="3" t="n">
-        <v>6.64</v>
+        <v>6.41</v>
       </c>
       <c r="U34" s="3" t="n">
-        <v>6.48</v>
+        <v>6.38</v>
       </c>
       <c r="V34" s="3" t="n">
-        <v>6.79</v>
+        <v>6.57</v>
       </c>
       <c r="W34" s="3" t="n">
-        <v>6.4</v>
+        <v>6.43</v>
       </c>
       <c r="X34" s="3" t="n">
         <v>5.86</v>
@@ -3346,10 +3346,10 @@
         <v>0.8</v>
       </c>
       <c r="D36" s="3" t="n">
-        <v>0.59</v>
+        <v>0.5</v>
       </c>
       <c r="E36" s="3" t="n">
-        <v>0.52</v>
+        <v>0.47</v>
       </c>
       <c r="F36" s="3" t="n">
         <v>0</v>
@@ -3391,19 +3391,19 @@
         <v>0</v>
       </c>
       <c r="S36" s="3" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="T36" s="3" t="n">
         <v>0.35</v>
       </c>
-      <c r="T36" s="3" t="n">
+      <c r="U36" s="3" t="n">
         <v>0.36</v>
       </c>
-      <c r="U36" s="3" t="n">
-        <v>0.35</v>
-      </c>
       <c r="V36" s="3" t="n">
-        <v>0.47</v>
+        <v>0.34</v>
       </c>
       <c r="W36" s="3" t="n">
-        <v>0.36</v>
+        <v>0.37</v>
       </c>
       <c r="X36" s="3" t="n">
         <v>0</v>
@@ -3430,10 +3430,10 @@
         <v>10.39</v>
       </c>
       <c r="D37" s="3" t="n">
-        <v>18.21</v>
+        <v>18.05</v>
       </c>
       <c r="E37" s="3" t="n">
-        <v>0</v>
+        <v>20.24</v>
       </c>
       <c r="F37" s="3" t="n">
         <v>0</v>
@@ -3457,10 +3457,10 @@
         <v>0</v>
       </c>
       <c r="M37" s="3" t="n">
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
       <c r="N37" s="3" t="n">
-        <v>0.16</v>
+        <v>0.11</v>
       </c>
       <c r="O37" s="3" t="n">
         <v>19.65</v>
@@ -3598,13 +3598,13 @@
         <v>15.1</v>
       </c>
       <c r="D39" s="3" t="n">
-        <v>99</v>
+        <v>7.04</v>
       </c>
       <c r="E39" s="3" t="n">
-        <v>155</v>
+        <v>105.2</v>
       </c>
       <c r="F39" s="3" t="n">
-        <v>155</v>
+        <v>75</v>
       </c>
       <c r="G39" s="3" t="n">
         <v>155</v>
@@ -3643,19 +3643,19 @@
         <v>0</v>
       </c>
       <c r="S39" s="3" t="n">
-        <v>6.04</v>
+        <v>6.17</v>
       </c>
       <c r="T39" s="3" t="n">
-        <v>6.46</v>
+        <v>6.22</v>
       </c>
       <c r="U39" s="3" t="n">
-        <v>6.29</v>
+        <v>6.18</v>
       </c>
       <c r="V39" s="3" t="n">
-        <v>6.5</v>
+        <v>6.41</v>
       </c>
       <c r="W39" s="3" t="n">
-        <v>6.19</v>
+        <v>6.21</v>
       </c>
       <c r="X39" s="3" t="n">
         <v>0</v>
@@ -3766,10 +3766,10 @@
         <v>0.4</v>
       </c>
       <c r="D41" s="3" t="n">
-        <v>0.11</v>
+        <v>0.23</v>
       </c>
       <c r="E41" s="3" t="n">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
       <c r="F41" s="3" t="n">
         <v>0</v>
@@ -3820,10 +3820,10 @@
         <v>0.16</v>
       </c>
       <c r="V41" s="3" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="W41" s="3" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="X41" s="3" t="n">
         <v>0</v>
@@ -3850,13 +3850,13 @@
         <v>0</v>
       </c>
       <c r="D42" s="3" t="n">
-        <v>92.31999999999999</v>
+        <v>0</v>
       </c>
       <c r="E42" s="3" t="n">
-        <v>148.8</v>
+        <v>98.7</v>
       </c>
       <c r="F42" s="3" t="n">
-        <v>155</v>
+        <v>75</v>
       </c>
       <c r="G42" s="3" t="n">
         <v>155</v>
@@ -4018,10 +4018,10 @@
         <v>14.79</v>
       </c>
       <c r="D44" s="3" t="n">
-        <v>6.5</v>
+        <v>6.87</v>
       </c>
       <c r="E44" s="3" t="n">
-        <v>5.99</v>
+        <v>6.34</v>
       </c>
       <c r="F44" s="3" t="n">
         <v>0</v>
@@ -4063,19 +4063,19 @@
         <v>0</v>
       </c>
       <c r="S44" s="3" t="n">
-        <v>5.88</v>
+        <v>6</v>
       </c>
       <c r="T44" s="3" t="n">
-        <v>6.3</v>
+        <v>6.07</v>
       </c>
       <c r="U44" s="3" t="n">
-        <v>6.14</v>
+        <v>6.04</v>
       </c>
       <c r="V44" s="3" t="n">
-        <v>6.34</v>
+        <v>6.24</v>
       </c>
       <c r="W44" s="3" t="n">
-        <v>6.03</v>
+        <v>6.06</v>
       </c>
       <c r="X44" s="3" t="n">
         <v>0</v>
@@ -4186,10 +4186,10 @@
         <v>0.1</v>
       </c>
       <c r="D46" s="3" t="n">
-        <v>-0.07000000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="E46" s="3" t="n">
-        <v>-0.02</v>
+        <v>0.04</v>
       </c>
       <c r="F46" s="3" t="n">
         <v>0</v>
@@ -4438,10 +4438,10 @@
         <v>13.98</v>
       </c>
       <c r="D49" s="3" t="n">
-        <v>5.95</v>
+        <v>6.49</v>
       </c>
       <c r="E49" s="3" t="n">
-        <v>5.7</v>
+        <v>5.97</v>
       </c>
       <c r="F49" s="3" t="n">
         <v>0</v>
@@ -4483,19 +4483,19 @@
         <v>0</v>
       </c>
       <c r="S49" s="3" t="n">
-        <v>5.35</v>
+        <v>5.46</v>
       </c>
       <c r="T49" s="3" t="n">
-        <v>5.72</v>
+        <v>5.5</v>
       </c>
       <c r="U49" s="3" t="n">
-        <v>5.59</v>
+        <v>5.49</v>
       </c>
       <c r="V49" s="3" t="n">
-        <v>5.76</v>
+        <v>5.69</v>
       </c>
       <c r="W49" s="3" t="n">
-        <v>5.49</v>
+        <v>5.51</v>
       </c>
       <c r="X49" s="3" t="n">
         <v>0</v>
@@ -4606,10 +4606,10 @@
         <v>-0.72</v>
       </c>
       <c r="D51" s="3" t="n">
-        <v>-0.62</v>
+        <v>-0.33</v>
       </c>
       <c r="E51" s="3" t="n">
-        <v>-0.31</v>
+        <v>-0.32</v>
       </c>
       <c r="F51" s="3" t="n">
         <v>0</v>
@@ -4651,16 +4651,16 @@
         <v>0</v>
       </c>
       <c r="S51" s="3" t="n">
-        <v>-0.54</v>
+        <v>-0.55</v>
       </c>
       <c r="T51" s="3" t="n">
-        <v>-0.57</v>
+        <v>-0.55</v>
       </c>
       <c r="U51" s="3" t="n">
         <v>-0.54</v>
       </c>
       <c r="V51" s="3" t="n">
-        <v>-0.5600000000000001</v>
+        <v>-0.55</v>
       </c>
       <c r="W51" s="3" t="n">
         <v>-0.55</v>
@@ -4858,10 +4858,10 @@
         <v>13.42</v>
       </c>
       <c r="D54" s="3" t="n">
-        <v>6.2</v>
+        <v>6.22</v>
       </c>
       <c r="E54" s="3" t="n">
-        <v>5.68</v>
+        <v>5.96</v>
       </c>
       <c r="F54" s="3" t="n">
         <v>0</v>
@@ -4903,19 +4903,19 @@
         <v>0</v>
       </c>
       <c r="S54" s="3" t="n">
-        <v>5.43</v>
+        <v>5.41</v>
       </c>
       <c r="T54" s="3" t="n">
+        <v>5.59</v>
+      </c>
+      <c r="U54" s="3" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="V54" s="3" t="n">
+        <v>5.64</v>
+      </c>
+      <c r="W54" s="3" t="n">
         <v>5.61</v>
-      </c>
-      <c r="U54" s="3" t="n">
-        <v>5.67</v>
-      </c>
-      <c r="V54" s="3" t="n">
-        <v>5.66</v>
-      </c>
-      <c r="W54" s="3" t="n">
-        <v>5.56</v>
       </c>
       <c r="X54" s="3" t="n">
         <v>0</v>
@@ -5026,7 +5026,7 @@
         <v>-1.27</v>
       </c>
       <c r="D56" s="3" t="n">
-        <v>-0.37</v>
+        <v>-0.6</v>
       </c>
       <c r="E56" s="3" t="n">
         <v>-0.33</v>
@@ -5071,19 +5071,19 @@
         <v>0</v>
       </c>
       <c r="S56" s="3" t="n">
-        <v>-0.46</v>
+        <v>-0.6</v>
       </c>
       <c r="T56" s="3" t="n">
-        <v>-0.67</v>
+        <v>-0.47</v>
       </c>
       <c r="U56" s="3" t="n">
-        <v>-0.46</v>
+        <v>-0.62</v>
       </c>
       <c r="V56" s="3" t="n">
-        <v>-0.67</v>
+        <v>-0.6</v>
       </c>
       <c r="W56" s="3" t="n">
-        <v>-0.48</v>
+        <v>-0.44</v>
       </c>
       <c r="X56" s="3" t="n">
         <v>0</v>
@@ -5278,10 +5278,10 @@
         <v>15.11</v>
       </c>
       <c r="D59" s="3" t="n">
-        <v>6.62</v>
+        <v>7.02</v>
       </c>
       <c r="E59" s="3" t="n">
-        <v>6.1</v>
+        <v>6.47</v>
       </c>
       <c r="F59" s="3" t="n">
         <v>0</v>
@@ -5323,19 +5323,19 @@
         <v>0</v>
       </c>
       <c r="S59" s="3" t="n">
-        <v>6</v>
+        <v>6.12</v>
       </c>
       <c r="T59" s="3" t="n">
-        <v>6.41</v>
+        <v>6.18</v>
       </c>
       <c r="U59" s="3" t="n">
-        <v>6.25</v>
+        <v>6.15</v>
       </c>
       <c r="V59" s="3" t="n">
-        <v>6.45</v>
+        <v>6.37</v>
       </c>
       <c r="W59" s="3" t="n">
-        <v>6.14</v>
+        <v>6.17</v>
       </c>
       <c r="X59" s="3" t="n">
         <v>0</v>
@@ -5446,10 +5446,10 @@
         <v>0.42</v>
       </c>
       <c r="D61" s="3" t="n">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="E61" s="3" t="n">
-        <v>0.09</v>
+        <v>0.18</v>
       </c>
       <c r="F61" s="3" t="n">
         <v>0</v>
@@ -5491,13 +5491,13 @@
         <v>0</v>
       </c>
       <c r="S61" s="3" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="T61" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="U61" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="V61" s="3" t="n">
         <v>0.13</v>
@@ -5698,10 +5698,10 @@
         <v>15.26</v>
       </c>
       <c r="D64" s="3" t="n">
-        <v>6.57</v>
+        <v>7.09</v>
       </c>
       <c r="E64" s="3" t="n">
-        <v>6.15</v>
+        <v>6.54</v>
       </c>
       <c r="F64" s="3" t="n">
         <v>0</v>
@@ -5743,19 +5743,19 @@
         <v>0</v>
       </c>
       <c r="S64" s="3" t="n">
-        <v>6.07</v>
+        <v>6.2</v>
       </c>
       <c r="T64" s="3" t="n">
-        <v>6.5</v>
+        <v>6.26</v>
       </c>
       <c r="U64" s="3" t="n">
-        <v>6.33</v>
+        <v>6.22</v>
       </c>
       <c r="V64" s="3" t="n">
-        <v>6.53</v>
+        <v>6.45</v>
       </c>
       <c r="W64" s="3" t="n">
-        <v>6.22</v>
+        <v>6.24</v>
       </c>
       <c r="X64" s="3" t="n">
         <v>0</v>
@@ -5866,10 +5866,10 @@
         <v>0.57</v>
       </c>
       <c r="D66" s="3" t="n">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="E66" s="3" t="n">
-        <v>0.14</v>
+        <v>0.25</v>
       </c>
       <c r="F66" s="3" t="n">
         <v>0</v>
@@ -6121,7 +6121,7 @@
         <v>55</v>
       </c>
       <c r="E69" s="3" t="n">
-        <v>6.13</v>
+        <v>35</v>
       </c>
       <c r="F69" s="3" t="n">
         <v>0</v>
@@ -6163,19 +6163,19 @@
         <v>0</v>
       </c>
       <c r="S69" s="3" t="n">
-        <v>6.03</v>
+        <v>6.15</v>
       </c>
       <c r="T69" s="3" t="n">
-        <v>6.45</v>
+        <v>6.22</v>
       </c>
       <c r="U69" s="3" t="n">
-        <v>6.28</v>
+        <v>6.18</v>
       </c>
       <c r="V69" s="3" t="n">
-        <v>6.48</v>
+        <v>6.4</v>
       </c>
       <c r="W69" s="3" t="n">
-        <v>6.18</v>
+        <v>6.2</v>
       </c>
       <c r="X69" s="3" t="n">
         <v>0</v>
@@ -6286,10 +6286,10 @@
         <v>0.61</v>
       </c>
       <c r="D71" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.31</v>
       </c>
       <c r="E71" s="3" t="n">
-        <v>0.12</v>
+        <v>0.27</v>
       </c>
       <c r="F71" s="3" t="n">
         <v>0</v>
@@ -6331,13 +6331,13 @@
         <v>0</v>
       </c>
       <c r="S71" s="3" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="T71" s="3" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="U71" s="3" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="V71" s="3" t="n">
         <v>0.16</v>
@@ -6370,10 +6370,10 @@
         <v>29.69</v>
       </c>
       <c r="D72" s="3" t="n">
-        <v>48.36</v>
+        <v>47.87</v>
       </c>
       <c r="E72" s="3" t="n">
-        <v>0</v>
+        <v>28.44</v>
       </c>
       <c r="F72" s="3" t="n">
         <v>0</v>
@@ -6538,10 +6538,10 @@
         <v>14.08</v>
       </c>
       <c r="D74" s="3" t="n">
-        <v>6.24</v>
+        <v>6.53</v>
       </c>
       <c r="E74" s="3" t="n">
-        <v>5.74</v>
+        <v>6.01</v>
       </c>
       <c r="F74" s="3" t="n">
         <v>0</v>
@@ -6583,19 +6583,19 @@
         <v>0</v>
       </c>
       <c r="S74" s="3" t="n">
-        <v>5.57</v>
+        <v>5.69</v>
       </c>
       <c r="T74" s="3" t="n">
-        <v>5.95</v>
+        <v>5.73</v>
       </c>
       <c r="U74" s="3" t="n">
-        <v>5.8</v>
+        <v>5.7</v>
       </c>
       <c r="V74" s="3" t="n">
-        <v>5.99</v>
+        <v>5.91</v>
       </c>
       <c r="W74" s="3" t="n">
-        <v>5.71</v>
+        <v>5.73</v>
       </c>
       <c r="X74" s="3" t="n">
         <v>0</v>
@@ -6706,10 +6706,10 @@
         <v>-0.62</v>
       </c>
       <c r="D76" s="3" t="n">
-        <v>-0.33</v>
+        <v>-0.29</v>
       </c>
       <c r="E76" s="3" t="n">
-        <v>-0.27</v>
+        <v>-0.28</v>
       </c>
       <c r="F76" s="3" t="n">
         <v>0</v>
@@ -6751,16 +6751,16 @@
         <v>0</v>
       </c>
       <c r="S76" s="3" t="n">
-        <v>-0.31</v>
+        <v>-0.32</v>
       </c>
       <c r="T76" s="3" t="n">
-        <v>-0.33</v>
+        <v>-0.32</v>
       </c>
       <c r="U76" s="3" t="n">
         <v>-0.32</v>
       </c>
       <c r="V76" s="3" t="n">
-        <v>-0.34</v>
+        <v>-0.33</v>
       </c>
       <c r="W76" s="3" t="n">
         <v>-0.33</v>
@@ -6958,64 +6958,64 @@
         <v>14.69</v>
       </c>
       <c r="D79" s="3" t="n">
-        <v>6.57</v>
+        <v>6.82</v>
       </c>
       <c r="E79" s="3" t="n">
+        <v>6.29</v>
+      </c>
+      <c r="F79" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H79" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J79" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K79" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L79" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M79" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N79" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O79" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P79" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q79" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R79" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S79" s="3" t="n">
         <v>6.01</v>
       </c>
-      <c r="F79" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G79" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H79" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I79" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J79" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K79" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L79" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M79" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N79" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O79" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P79" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q79" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R79" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S79" s="3" t="n">
-        <v>5.89</v>
-      </c>
       <c r="T79" s="3" t="n">
-        <v>6.28</v>
+        <v>6.06</v>
       </c>
       <c r="U79" s="3" t="n">
-        <v>6.13</v>
+        <v>6.02</v>
       </c>
       <c r="V79" s="3" t="n">
-        <v>6.32</v>
+        <v>6.24</v>
       </c>
       <c r="W79" s="3" t="n">
-        <v>6.03</v>
+        <v>6.06</v>
       </c>
       <c r="X79" s="3" t="n">
         <v>0</v>
@@ -7378,10 +7378,10 @@
         <v>12.84</v>
       </c>
       <c r="D84" s="3" t="n">
-        <v>6.27</v>
+        <v>5.94</v>
       </c>
       <c r="E84" s="3" t="n">
-        <v>5.81</v>
+        <v>6.04</v>
       </c>
       <c r="F84" s="3" t="n">
         <v>0</v>
@@ -7423,19 +7423,19 @@
         <v>0</v>
       </c>
       <c r="S84" s="3" t="n">
-        <v>5.45</v>
+        <v>5.21</v>
       </c>
       <c r="T84" s="3" t="n">
-        <v>5.34</v>
+        <v>5.66</v>
       </c>
       <c r="U84" s="3" t="n">
-        <v>5.78</v>
+        <v>5.19</v>
       </c>
       <c r="V84" s="3" t="n">
-        <v>5.46</v>
+        <v>5.56</v>
       </c>
       <c r="W84" s="3" t="n">
-        <v>5.6</v>
+        <v>5.73</v>
       </c>
       <c r="X84" s="3" t="n">
         <v>0</v>
@@ -7546,10 +7546,10 @@
         <v>-1.86</v>
       </c>
       <c r="D86" s="3" t="n">
-        <v>-0.3</v>
+        <v>-0.88</v>
       </c>
       <c r="E86" s="3" t="n">
-        <v>-0.2</v>
+        <v>-0.25</v>
       </c>
       <c r="F86" s="3" t="n">
         <v>0</v>
@@ -7591,19 +7591,19 @@
         <v>0</v>
       </c>
       <c r="S86" s="3" t="n">
-        <v>-0.44</v>
+        <v>-0.8</v>
       </c>
       <c r="T86" s="3" t="n">
-        <v>-0.9399999999999999</v>
+        <v>-0.4</v>
       </c>
       <c r="U86" s="3" t="n">
-        <v>-0.35</v>
+        <v>-0.84</v>
       </c>
       <c r="V86" s="3" t="n">
-        <v>-0.86</v>
+        <v>-0.68</v>
       </c>
       <c r="W86" s="3" t="n">
-        <v>-0.43</v>
+        <v>-0.33</v>
       </c>
       <c r="X86" s="3" t="n">
         <v>0</v>
@@ -7798,13 +7798,13 @@
         <v>15.37</v>
       </c>
       <c r="D89" s="3" t="n">
-        <v>53.05</v>
+        <v>53.06</v>
       </c>
       <c r="E89" s="3" t="n">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="F89" s="3" t="n">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="G89" s="3" t="n">
         <v>32</v>
@@ -7843,10 +7843,10 @@
         <v>0</v>
       </c>
       <c r="S89" s="3" t="n">
-        <v>6.13</v>
+        <v>6.26</v>
       </c>
       <c r="T89" s="3" t="n">
-        <v>6.54</v>
+        <v>6.31</v>
       </c>
       <c r="U89" s="3" t="n">
         <v>115</v>
@@ -7966,10 +7966,10 @@
         <v>0.67</v>
       </c>
       <c r="D91" s="3" t="n">
-        <v>0.22</v>
+        <v>0.34</v>
       </c>
       <c r="E91" s="3" t="n">
-        <v>0.31</v>
+        <v>0.32</v>
       </c>
       <c r="F91" s="3" t="n">
         <v>0</v>
@@ -8011,19 +8011,19 @@
         <v>0</v>
       </c>
       <c r="S91" s="3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="T91" s="3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="U91" s="3" t="n">
         <v>0.24</v>
       </c>
-      <c r="T91" s="3" t="n">
-        <v>0.26</v>
-      </c>
-      <c r="U91" s="3" t="n">
+      <c r="V91" s="3" t="n">
         <v>0.25</v>
       </c>
-      <c r="V91" s="3" t="n">
-        <v>0.27</v>
-      </c>
       <c r="W91" s="3" t="n">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="X91" s="3" t="n">
         <v>0</v>
@@ -8050,13 +8050,13 @@
         <v>0</v>
       </c>
       <c r="D92" s="3" t="n">
-        <v>46.26</v>
+        <v>45.9</v>
       </c>
       <c r="E92" s="3" t="n">
-        <v>27.68</v>
+        <v>68.39</v>
       </c>
       <c r="F92" s="3" t="n">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="G92" s="3" t="n">
         <v>32</v>
@@ -8101,13 +8101,13 @@
         <v>0</v>
       </c>
       <c r="U92" s="3" t="n">
-        <v>108.62</v>
+        <v>108.73</v>
       </c>
       <c r="V92" s="3" t="n">
-        <v>108.41</v>
+        <v>108.51</v>
       </c>
       <c r="W92" s="3" t="n">
-        <v>36.72</v>
+        <v>36.7</v>
       </c>
       <c r="X92" s="3" t="n">
         <v>0</v>

</xml_diff>